<commit_message>
return file name to fe
</commit_message>
<xml_diff>
--- a/resources/static/files/Báo cáo công việc.xlsx
+++ b/resources/static/files/Báo cáo công việc.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="248">
   <si>
     <t>STT</t>
   </si>
@@ -53,30 +53,6 @@
   </si>
   <si>
     <t>20.00</t>
-  </si>
-  <si>
-    <t>26-12-2022</t>
-  </si>
-  <si>
-    <t>Tìm kiếm thành viên phụ trách, lập ý tưởng kèm phác thảo Docca dựa trên các app Pharmacity, Flo, Thể dục</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669864331963_1.JPG, </t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>13-12-2022</t>
-  </si>
-  <si>
-    <t>Tìm và lấy lại thông tin domain Boxstore</t>
-  </si>
-  <si>
-    <t>20-12-2022</t>
-  </si>
-  <si>
-    <t>Đào tạo digi tiếp nhận và sử dụng</t>
   </si>
   <si>
     <t>19-12-2022</t>
@@ -86,12 +62,36 @@
 https://docca.sweetsica.com</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>26-12-2022</t>
+  </si>
+  <si>
+    <t>Tìm kiếm thành viên phụ trách, lập ý tưởng kèm phác thảo Docca dựa trên các app Pharmacity, Flo, Thể dục</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669864331963_1.JPG, </t>
+  </si>
+  <si>
     <t>17-12-2022</t>
   </si>
   <si>
     <t>Lên giao diện Docca website</t>
   </si>
   <si>
+    <t>20-12-2022</t>
+  </si>
+  <si>
+    <t>Đào tạo digi tiếp nhận và sử dụng</t>
+  </si>
+  <si>
+    <t>13-12-2022</t>
+  </si>
+  <si>
+    <t>Tìm và lấy lại thông tin domain Boxstore</t>
+  </si>
+  <si>
     <t>Vận hành hệ thống phần mềm</t>
   </si>
   <si>
@@ -101,25 +101,37 @@
     <t>24.00</t>
   </si>
   <si>
+    <t>22-12-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xuất 205.000 mã QR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669863237817_Danh-sÃ¡ch-mÃ£-QR-Kinder-Immune-tá»«-395006-Äáº¿n-405005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863237818_Danh-sÃ¡ch-mÃ£-QR-Kinder-Omega-tá»«-415006-Äáº¿n-420005-ngÃ y-24-11-2022.xlsx, </t>
+  </si>
+  <si>
+    <t>21-12-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669863265732_Danh-sÃ¡ch-mÃ£-QR-Kinder-Active-tá»«-375006-Äáº¿n-385005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863265734_Danh-sÃ¡ch-mÃ£-QR-Kinder-Calciovin-tá»«-385006-Äáº¿n-395005-ngÃ y-24-11-2022.xlsx, </t>
+  </si>
+  <si>
     <t>Sửa lại code logic, lỗi không hiện tên sản phẩm đã quét</t>
   </si>
   <si>
     <t xml:space="preserve">localhost:3002/uploads/1669864249977_1.JPG, </t>
   </si>
   <si>
-    <t>21-12-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xuất 205.000 mã QR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669863265732_Danh-sÃ¡ch-mÃ£-QR-Kinder-Active-tá»«-375006-Äáº¿n-385005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863265734_Danh-sÃ¡ch-mÃ£-QR-Kinder-Calciovin-tá»«-385006-Äáº¿n-395005-ngÃ y-24-11-2022.xlsx, </t>
-  </si>
-  <si>
-    <t>22-12-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669863237817_Danh-sÃ¡ch-mÃ£-QR-Kinder-Immune-tá»«-395006-Äáº¿n-405005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863237818_Danh-sÃ¡ch-mÃ£-QR-Kinder-Omega-tá»«-415006-Äáº¿n-420005-ngÃ y-24-11-2022.xlsx, </t>
+    <t>Backup dữ liệu nhiệm vụ phòng mua hàng và cung ứng DWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669862793520_Danh má»¥c new.xlsx, </t>
+  </si>
+  <si>
+    <t>24-12-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669863201162_Danh-sÃ¡ch-mÃ£-QR-Omega-3-Folic-Axit-tá»«-440006-Äáº¿n-450005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863201175_Danh-sÃ¡ch-mÃ£-QR-Prostacalm-tá»«-450006-Äáº¿n-460005-ngÃ y-24-11-2022.xlsx, </t>
   </si>
   <si>
     <t>23-12-2022</t>
@@ -128,18 +140,6 @@
     <t xml:space="preserve">localhost:3002/uploads/1669863221151_Danh-sÃ¡ch-mÃ£-QR-Kinder-Thymepect-tá»«-420006-Äáº¿n-430005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863221154_Danh-sÃ¡ch-mÃ£-QR-Liver-Complex-tá»«-430006-Äáº¿n-450005-ngÃ y-24-11-2022.xlsx, </t>
   </si>
   <si>
-    <t>24-12-2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669863201162_Danh-sÃ¡ch-mÃ£-QR-Omega-3-Folic-Axit-tá»«-440006-Äáº¿n-450005-ngÃ y-24-11-2022.xlsx, localhost:3002/uploads/1669863201175_Danh-sÃ¡ch-mÃ£-QR-Prostacalm-tá»«-450006-Äáº¿n-460005-ngÃ y-24-11-2022.xlsx, </t>
-  </si>
-  <si>
-    <t>Backup dữ liệu nhiệm vụ phòng mua hàng và cung ứng DWT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669862793520_Danh má»¥c new.xlsx, </t>
-  </si>
-  <si>
     <t>Xử lý các vấn đề kỹ thuật phát sinh</t>
   </si>
   <si>
@@ -149,13 +149,8 @@
     <t>36.00</t>
   </si>
   <si>
-    <t>30-12-2022</t>
-  </si>
-  <si>
-    <t>Tiếp nhận quản trị Base</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669865279756_3.png, </t>
+    <t xml:space="preserve">Sửa giao diện đào tạo trực tuyến 
+https://elearning.doppelherz.vn</t>
   </si>
   <si>
     <t>16-12-2022</t>
@@ -180,6 +175,15 @@
     <t xml:space="preserve">localhost:3002/uploads/1669865418343_3.png, </t>
   </si>
   <si>
+    <t>30-12-2022</t>
+  </si>
+  <si>
+    <t>Tiếp nhận quản trị Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669865279756_3.png, </t>
+  </si>
+  <si>
     <t>29-12-2022</t>
   </si>
   <si>
@@ -195,10 +199,6 @@
     <t xml:space="preserve">localhost:3002/uploads/1669864925499_3.png, </t>
   </si>
   <si>
-    <t xml:space="preserve">Sửa giao diện đào tạo trực tuyến 
-https://elearning.doppelherz.vn</t>
-  </si>
-  <si>
     <t>Nhận thông tin sửa đào tạo online</t>
   </si>
   <si>
@@ -211,6 +211,36 @@
     <t>32.00</t>
   </si>
   <si>
+    <t>12-12-2022</t>
+  </si>
+  <si>
+    <t>Backup dữ liệu mail admin9, ducnh, sam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669864093518_1.JPG, </t>
+  </si>
+  <si>
+    <t>Tiếp nhận quản trị Email, kiểm tra và đồng bộ nhóm mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669865346470_3.png, </t>
+  </si>
+  <si>
+    <t>15-12-2022</t>
+  </si>
+  <si>
+    <t>Rà soát, sao lưu dữ liệu dungnq, trinhbd, sêding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669864206286_1.JPG, </t>
+  </si>
+  <si>
+    <t>Check và tài khoản Phạm Thùy Linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669864047880_1.JPG, </t>
+  </si>
+  <si>
     <t>11-12-2022</t>
   </si>
   <si>
@@ -220,36 +250,6 @@
     <t xml:space="preserve">localhost:3002/uploads/1669863947828_1.JPG, </t>
   </si>
   <si>
-    <t>Check và tài khoản Phạm Thùy Linh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669864047880_1.JPG, </t>
-  </si>
-  <si>
-    <t>12-12-2022</t>
-  </si>
-  <si>
-    <t>Backup dữ liệu mail admin9, ducnh, sam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669864093518_1.JPG, </t>
-  </si>
-  <si>
-    <t>15-12-2022</t>
-  </si>
-  <si>
-    <t>Rà soát, sao lưu dữ liệu dungnq, trinhbd, sêding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669864206286_1.JPG, </t>
-  </si>
-  <si>
-    <t>Tiếp nhận quản trị Email, kiểm tra và đồng bộ nhóm mail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669865346470_3.png, </t>
-  </si>
-  <si>
     <t>Backup dữ liệu</t>
   </si>
   <si>
@@ -271,19 +271,19 @@
     <t>Tìm kiếm nhà cung cấp</t>
   </si>
   <si>
+    <t>02-11-2022</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost:3002/uploads/1669190259381_giao-huu-bong-da.cpp, localhost:3002/uploads/1669190259381_tuyen-nhan-su.cpp, </t>
+  </si>
+  <si>
     <t>01-11-2022</t>
   </si>
   <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>02-11-2022</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1669190259381_giao-huu-bong-da.cpp, localhost:3002/uploads/1669190259381_tuyen-nhan-su.cpp, </t>
   </si>
   <si>
     <t>Thương lượng ký kết hợp đồng</t>
@@ -532,13 +532,13 @@
     <t>10.00</t>
   </si>
   <si>
+    <t xml:space="preserve">localhost:3002/uploads/1670165654267_bingsu-logo.jpg, </t>
+  </si>
+  <si>
     <t>01-12-2022</t>
   </si>
   <si>
     <t>Báo cáo tháng 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost:3002/uploads/1670165654267_bingsu-logo.jpg, </t>
   </si>
   <si>
     <t>Giám sát, đôn đốc thực hiện kế hoạch, đánh giá KPI cho phòng</t>
@@ -1139,7 +1139,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J148"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1215,57 +1215,57 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -1274,30 +1274,30 @@
         <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
@@ -1306,30 +1306,30 @@
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>
@@ -1338,7 +1338,7 @@
         <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1364,42 +1364,42 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s">
         <v>33</v>
@@ -1407,31 +1407,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
         <v>34</v>
-      </c>
-      <c r="I9" t="s">
-        <v>32</v>
       </c>
       <c r="J9" t="s">
         <v>35</v>
@@ -1439,31 +1439,31 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>36</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
       </c>
       <c r="J10" t="s">
         <v>37</v>
@@ -1471,31 +1471,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J11" t="s">
         <v>39</v>
@@ -1503,31 +1503,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
@@ -1556,269 +1556,269 @@
         <v>6</v>
       </c>
       <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
         <v>45</v>
       </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
       <c r="J13" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
         <v>52</v>
-      </c>
-      <c r="I17" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" t="s">
         <v>55</v>
-      </c>
-      <c r="I18" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="I19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" t="s">
         <v>58</v>
-      </c>
-      <c r="J19" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" t="s">
-        <v>34</v>
-      </c>
       <c r="I20" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" t="s">
         <v>60</v>
-      </c>
-      <c r="J20" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I21" t="s">
         <v>61</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1855,28 +1855,28 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I23" t="s">
         <v>68</v>
@@ -1887,25 +1887,25 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
         <v>70</v>
@@ -1919,60 +1919,60 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" t="s">
         <v>73</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>74</v>
-      </c>
-      <c r="J25" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="I26" t="s">
         <v>76</v>
@@ -2004,7 +2004,7 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I27" t="s">
         <v>80</v>
@@ -2015,28 +2015,28 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
         <v>17</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" t="s">
-        <v>14</v>
       </c>
       <c r="I28" t="s">
         <v>82</v>
@@ -2074,39 +2074,39 @@
         <v>86</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J30" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2138,30 +2138,30 @@
         <v>92</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" t="s">
         <v>93</v>
@@ -2175,25 +2175,25 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" t="s">
         <v>96</v>
@@ -2202,7 +2202,7 @@
         <v>97</v>
       </c>
       <c r="J33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2271,25 +2271,25 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36" t="s">
         <v>110</v>
@@ -2298,7 +2298,7 @@
         <v>111</v>
       </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2324,10 +2324,10 @@
         <v>8</v>
       </c>
       <c r="H37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>117</v>
       </c>
       <c r="J38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2388,33 +2388,33 @@
         <v>121</v>
       </c>
       <c r="I39" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H40" t="s">
         <v>93</v>
@@ -2484,30 +2484,30 @@
         <v>130</v>
       </c>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" t="s">
         <v>131</v>
@@ -2516,30 +2516,30 @@
         <v>132</v>
       </c>
       <c r="J43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H44" t="s">
         <v>133</v>
@@ -2571,10 +2571,10 @@
         <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>138</v>
       </c>
       <c r="J46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>139</v>
       </c>
       <c r="J47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>141</v>
       </c>
       <c r="J48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>143</v>
       </c>
       <c r="J49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
         <v>145</v>
       </c>
       <c r="J50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2760,10 +2760,10 @@
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2789,10 +2789,10 @@
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2818,10 +2818,10 @@
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
         <v>145</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2879,10 +2879,10 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2908,10 +2908,10 @@
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2937,10 +2937,10 @@
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2972,7 +2972,7 @@
         <v>147</v>
       </c>
       <c r="J58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2998,10 +2998,10 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3027,10 +3027,10 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3056,10 +3056,10 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3082,10 +3082,10 @@
         <v>12</v>
       </c>
       <c r="H62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3111,10 +3111,10 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3140,10 +3140,10 @@
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3169,10 +3169,10 @@
         <v>1</v>
       </c>
       <c r="H65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>149</v>
       </c>
       <c r="J66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3227,10 +3227,10 @@
         <v>12</v>
       </c>
       <c r="H67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3253,10 +3253,10 @@
         <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3279,10 +3279,10 @@
         <v>2</v>
       </c>
       <c r="H69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3305,10 +3305,10 @@
         <v>11</v>
       </c>
       <c r="H70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -3366,10 +3366,10 @@
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>159</v>
       </c>
       <c r="J73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3427,10 +3427,10 @@
         <v>1</v>
       </c>
       <c r="H74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3456,10 +3456,10 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -3485,45 +3485,45 @@
         <v>28</v>
       </c>
       <c r="H76" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I76" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H77" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I77" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3549,10 +3549,10 @@
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -3584,7 +3584,7 @@
         <v>165</v>
       </c>
       <c r="J79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3610,10 +3610,10 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3639,10 +3639,10 @@
         <v>1</v>
       </c>
       <c r="H81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I81" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3668,10 +3668,10 @@
         <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I82" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3697,10 +3697,10 @@
         <v>5</v>
       </c>
       <c r="H83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -3726,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I84" t="s">
         <v>167</v>
@@ -3758,45 +3758,45 @@
         <v>1</v>
       </c>
       <c r="H85" t="s">
+        <v>93</v>
+      </c>
+      <c r="I85" t="s">
+        <v>94</v>
+      </c>
+      <c r="J85" t="s">
         <v>171</v>
-      </c>
-      <c r="I85" t="s">
-        <v>172</v>
-      </c>
-      <c r="J85" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H86" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="I86" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="J86" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3822,10 +3822,10 @@
         <v>8</v>
       </c>
       <c r="H87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3851,10 +3851,10 @@
         <v>24</v>
       </c>
       <c r="H88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3880,10 +3880,10 @@
         <v>24</v>
       </c>
       <c r="H89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3909,10 +3909,10 @@
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3938,10 +3938,10 @@
         <v>1</v>
       </c>
       <c r="H91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3967,10 +3967,10 @@
         <v>1</v>
       </c>
       <c r="H92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I92" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3996,10 +3996,10 @@
         <v>5</v>
       </c>
       <c r="H93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I93" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4025,10 +4025,10 @@
         <v>2</v>
       </c>
       <c r="H94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I94" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4054,10 +4054,10 @@
         <v>6400</v>
       </c>
       <c r="H95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4083,10 +4083,10 @@
         <v>1</v>
       </c>
       <c r="H96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4112,10 +4112,10 @@
         <v>50</v>
       </c>
       <c r="H97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4141,10 +4141,10 @@
         <v>50</v>
       </c>
       <c r="H98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4170,10 +4170,10 @@
         <v>1</v>
       </c>
       <c r="H99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I99" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4199,10 +4199,10 @@
         <v>1</v>
       </c>
       <c r="H100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4228,10 +4228,10 @@
         <v>1</v>
       </c>
       <c r="H101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I101" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4257,10 +4257,10 @@
         <v>1</v>
       </c>
       <c r="H102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4286,10 +4286,10 @@
         <v>60</v>
       </c>
       <c r="H103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4315,10 +4315,10 @@
         <v>6000</v>
       </c>
       <c r="H104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4344,10 +4344,10 @@
         <v>100</v>
       </c>
       <c r="H105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I105" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4373,10 +4373,10 @@
         <v>1</v>
       </c>
       <c r="H106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I106" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4402,10 +4402,10 @@
         <v>1</v>
       </c>
       <c r="H107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4431,10 +4431,10 @@
         <v>1</v>
       </c>
       <c r="H108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4460,10 +4460,10 @@
         <v>1</v>
       </c>
       <c r="H109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4489,10 +4489,10 @@
         <v>5</v>
       </c>
       <c r="H110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4518,10 +4518,10 @@
         <v>1</v>
       </c>
       <c r="H111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4547,10 +4547,10 @@
         <v>1</v>
       </c>
       <c r="H112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4576,10 +4576,10 @@
         <v>2</v>
       </c>
       <c r="H113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I113" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4605,10 +4605,10 @@
         <v>1</v>
       </c>
       <c r="H114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
@@ -4640,7 +4640,7 @@
         <v>211</v>
       </c>
       <c r="J115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4666,10 +4666,10 @@
         <v>30</v>
       </c>
       <c r="H116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I116" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4695,10 +4695,10 @@
         <v>200</v>
       </c>
       <c r="H117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I117" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4724,10 +4724,10 @@
         <v>25</v>
       </c>
       <c r="H118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4753,10 +4753,10 @@
         <v>25</v>
       </c>
       <c r="H119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4782,10 +4782,10 @@
         <v>200</v>
       </c>
       <c r="H120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4811,10 +4811,10 @@
         <v>3000</v>
       </c>
       <c r="H121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I121" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4840,10 +4840,10 @@
         <v>100</v>
       </c>
       <c r="H122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I122" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4869,10 +4869,10 @@
         <v>300</v>
       </c>
       <c r="H123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4898,10 +4898,10 @@
         <v>5</v>
       </c>
       <c r="H124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I124" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4927,10 +4927,10 @@
         <v>100</v>
       </c>
       <c r="H125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I125" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4956,10 +4956,10 @@
         <v>2</v>
       </c>
       <c r="H126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I126" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4985,10 +4985,10 @@
         <v>4</v>
       </c>
       <c r="H127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -5014,10 +5014,10 @@
         <v>15</v>
       </c>
       <c r="H128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -5043,10 +5043,10 @@
         <v>1</v>
       </c>
       <c r="H129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I129" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5072,10 +5072,10 @@
         <v>1</v>
       </c>
       <c r="H130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -5101,10 +5101,10 @@
         <v>200</v>
       </c>
       <c r="H131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -5130,10 +5130,10 @@
         <v>2</v>
       </c>
       <c r="H132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I132" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -5159,10 +5159,10 @@
         <v>6</v>
       </c>
       <c r="H133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5188,10 +5188,10 @@
         <v>6</v>
       </c>
       <c r="H134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I134" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5217,10 +5217,10 @@
         <v>3</v>
       </c>
       <c r="H135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -5246,10 +5246,10 @@
         <v>4</v>
       </c>
       <c r="H136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5275,10 +5275,10 @@
         <v>1</v>
       </c>
       <c r="H137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I137" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5304,10 +5304,10 @@
         <v>1</v>
       </c>
       <c r="H138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I138" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -5333,10 +5333,10 @@
         <v>1</v>
       </c>
       <c r="H139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I139" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5362,10 +5362,10 @@
         <v>6000</v>
       </c>
       <c r="H140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I140" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5388,10 +5388,10 @@
         <v>1</v>
       </c>
       <c r="H141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5417,10 +5417,10 @@
         <v>1</v>
       </c>
       <c r="H142" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I142" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -5446,10 +5446,10 @@
         <v>1</v>
       </c>
       <c r="H143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5475,10 +5475,10 @@
         <v>1</v>
       </c>
       <c r="H144" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I144" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -5504,10 +5504,10 @@
         <v>1</v>
       </c>
       <c r="H145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -5533,10 +5533,10 @@
         <v>1</v>
       </c>
       <c r="H146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I146" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5562,10 +5562,39 @@
         <v>300</v>
       </c>
       <c r="H147" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I147" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>116</v>
+      </c>
+      <c r="B148" t="s">
+        <v>112</v>
+      </c>
+      <c r="C148" t="s">
+        <v>113</v>
+      </c>
+      <c r="D148" t="s">
+        <v>119</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>0.8</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+      <c r="H148" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>